<commit_message>
SR [2022-08-25]: Mgmt Excel parcing --> PS_Class meth for parsing XLS finished --> templ Qwr for PQ Record created
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Type</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Sergii Razumov</t>
   </si>
   <si>
-    <t>Ready By</t>
-  </si>
-  <si>
     <t>Internet Sales Amount</t>
   </si>
   <si>
@@ -70,6 +67,30 @@
   </si>
   <si>
     <t>A plan of the object to develop in the Sprint</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Ready %</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Comment </t>
+  </si>
+  <si>
+    <t>PM Comment</t>
+  </si>
+  <si>
+    <t>Waiting for data validation from EDA</t>
   </si>
 </sst>
 </file>
@@ -114,16 +135,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
@@ -141,14 +168,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:E8" totalsRowShown="0">
-  <autoFilter ref="A3:E8"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:I8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A3:I8"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Object"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Link to Specification" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" name="Developer"/>
-    <tableColumn id="5" name="Ready By" dataDxfId="0"/>
+    <tableColumn id="5" name="Due Date" dataDxfId="1"/>
+    <tableColumn id="6" name="Sprint"/>
+    <tableColumn id="7" name="Ready %"/>
+    <tableColumn id="8" name="Dev Comment "/>
+    <tableColumn id="9" name="PM Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,36 +460,50 @@
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -469,13 +514,22 @@
       <c r="E4" s="2">
         <v>44803</v>
       </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>0.85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -486,13 +540,19 @@
       <c r="E5" s="2">
         <v>44803</v>
       </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -503,13 +563,19 @@
       <c r="E6" s="2">
         <v>44803</v>
       </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -521,12 +587,12 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -539,6 +605,20 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G4:G8">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{90414F64-16F4-4DFF-91DA-BBBBF222D494}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C5" r:id="rId2"/>
@@ -547,9 +627,29 @@
     <hyperlink ref="C8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{90414F64-16F4-4DFF-91DA-BBBBF222D494}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4:G8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SR: minor changes to Mgm Qwr --> txt btw delimiters found
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -78,9 +78,6 @@
     <t>1,2,3</t>
   </si>
   <si>
-    <t>Ready %</t>
-  </si>
-  <si>
     <t>2,3</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Waiting for data validation from EDA</t>
+  </si>
+  <si>
+    <t>Ready pct</t>
   </si>
 </sst>
 </file>
@@ -149,10 +149,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,16 +168,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:I8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:I8" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:I8"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Object"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Link to Specification" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" name="Developer"/>
-    <tableColumn id="5" name="Due Date" dataDxfId="1"/>
+    <tableColumn id="5" name="Due Date" dataDxfId="0"/>
     <tableColumn id="6" name="Sprint"/>
-    <tableColumn id="7" name="Ready %"/>
+    <tableColumn id="7" name="Ready pct"/>
     <tableColumn id="8" name="Dev Comment "/>
     <tableColumn id="9" name="PM Comment"/>
   </tableColumns>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,13 +489,13 @@
         <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -521,7 +521,7 @@
         <v>0.85</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>44803</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>0.5</v>

</xml_diff>

<commit_message>
SR [2022-08-30] : PS Mgm Tbl + Minor visual chng 1. Combining of Qwr str
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -27,24 +27,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
     <t>Internet Sales</t>
   </si>
   <si>
-    <t>Link to Specification</t>
-  </si>
-  <si>
     <t>https://onedrive.live.com/view.aspx?resid=43FC8CA3B17868DD%21806&amp;id=documents&amp;wd=target%28VS%20Code.one%7C062DAB10-4A3E-4127-8D96-1AB4A4286FC7%2FDummyTask%3A%20Add%20Internet-Sales%7CC38A5B3B-DB39-4862-8800-09D041CB42B0%2F%29</t>
   </si>
   <si>
-    <t>Developer</t>
-  </si>
-  <si>
     <t>Sergii Razumov</t>
   </si>
   <si>
@@ -69,28 +57,40 @@
     <t>A plan of the object to develop in the Sprint</t>
   </si>
   <si>
-    <t>Due Date</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
     <t>1,2,3</t>
   </si>
   <si>
     <t>2,3</t>
   </si>
   <si>
-    <t xml:space="preserve">Dev Comment </t>
-  </si>
-  <si>
-    <t>PM Comment</t>
-  </si>
-  <si>
     <t>Waiting for data validation from EDA</t>
   </si>
   <si>
-    <t>Ready pct</t>
+    <t>01_Object</t>
+  </si>
+  <si>
+    <t>02_Type</t>
+  </si>
+  <si>
+    <t>03_Link to Specification</t>
+  </si>
+  <si>
+    <t>04_Developer</t>
+  </si>
+  <si>
+    <t>05_Due Date</t>
+  </si>
+  <si>
+    <t>06_Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08_Dev Comment </t>
+  </si>
+  <si>
+    <t>09_PM Comment</t>
+  </si>
+  <si>
+    <t>07_Ready for %</t>
   </si>
 </sst>
 </file>
@@ -171,15 +171,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:I8" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:I8"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Object"/>
-    <tableColumn id="2" name="Type"/>
-    <tableColumn id="3" name="Link to Specification" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Developer"/>
-    <tableColumn id="5" name="Due Date" dataDxfId="0"/>
-    <tableColumn id="6" name="Sprint"/>
-    <tableColumn id="7" name="Ready pct"/>
-    <tableColumn id="8" name="Dev Comment "/>
-    <tableColumn id="9" name="PM Comment"/>
+    <tableColumn id="1" name="01_Object"/>
+    <tableColumn id="2" name="02_Type"/>
+    <tableColumn id="3" name="03_Link to Specification" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="04_Developer"/>
+    <tableColumn id="5" name="05_Due Date" dataDxfId="0"/>
+    <tableColumn id="6" name="06_Sprint"/>
+    <tableColumn id="7" name="07_Ready for %"/>
+    <tableColumn id="8" name="08_Dev Comment "/>
+    <tableColumn id="9" name="09_PM Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,76 +466,76 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
       </c>
       <c r="E4" s="2">
         <v>44803</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>0.85</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
         <v>44803</v>
@@ -549,22 +549,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
         <v>44803</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -572,16 +572,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2">
         <v>44803</v>
@@ -589,16 +589,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
         <v>44803</v>

</xml_diff>

<commit_message>
SR [2022-08-30]: RgEx: multiline replcmt finished
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -90,7 +90,7 @@
     <t>09_PM Comment</t>
   </si>
   <si>
-    <t>07_Ready for %</t>
+    <t>07_Ready for pct</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
     <tableColumn id="4" name="04_Developer"/>
     <tableColumn id="5" name="05_Due Date" dataDxfId="0"/>
     <tableColumn id="6" name="06_Sprint"/>
-    <tableColumn id="7" name="07_Ready for %"/>
+    <tableColumn id="7" name="07_Ready for pct"/>
     <tableColumn id="8" name="08_Dev Comment "/>
     <tableColumn id="9" name="09_PM Comment"/>
   </tableColumns>

</xml_diff>

<commit_message>
SR [2022-08-31]: PS xls mgm prototype finished --> finished in .Net notebook
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Internet Sales</t>
   </si>
@@ -33,9 +33,6 @@
     <t>https://onedrive.live.com/view.aspx?resid=43FC8CA3B17868DD%21806&amp;id=documents&amp;wd=target%28VS%20Code.one%7C062DAB10-4A3E-4127-8D96-1AB4A4286FC7%2FDummyTask%3A%20Add%20Internet-Sales%7CC38A5B3B-DB39-4862-8800-09D041CB42B0%2F%29</t>
   </si>
   <si>
-    <t>Sergii Razumov</t>
-  </si>
-  <si>
     <t>Internet Sales Amount</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Waiting for data validation from EDA</t>
   </si>
   <si>
-    <t>01_Object</t>
-  </si>
-  <si>
     <t>02_Type</t>
   </si>
   <si>
@@ -78,19 +72,73 @@
     <t>04_Developer</t>
   </si>
   <si>
-    <t>05_Due Date</t>
-  </si>
-  <si>
-    <t>06_Sprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08_Dev Comment </t>
-  </si>
-  <si>
-    <t>09_PM Comment</t>
-  </si>
-  <si>
-    <t>07_Ready for pct</t>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Sergii_Razumov@epam.com</t>
+  </si>
+  <si>
+    <t>08_Status</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>To Start</t>
+  </si>
+  <si>
+    <t>UAT</t>
+  </si>
+  <si>
+    <t>implementing User Remarks</t>
+  </si>
+  <si>
+    <t>05_Tasks</t>
+  </si>
+  <si>
+    <t>JR-02</t>
+  </si>
+  <si>
+    <t>JR-03</t>
+  </si>
+  <si>
+    <t>JR-04</t>
+  </si>
+  <si>
+    <t>JR-05</t>
+  </si>
+  <si>
+    <t>JR-06</t>
+  </si>
+  <si>
+    <t>06_Due Date</t>
+  </si>
+  <si>
+    <t>07_Sprint</t>
+  </si>
+  <si>
+    <t>09_Ready for pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_Dev Comment </t>
+  </si>
+  <si>
+    <t>11_PM Comment</t>
+  </si>
+  <si>
+    <t>01_Object Name</t>
+  </si>
+  <si>
+    <t>JR-01, JR-15, JR-16/1</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>JR-07</t>
+  </si>
+  <si>
+    <t>Waiting for specification</t>
   </si>
 </sst>
 </file>
@@ -168,18 +216,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:I8" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:I8"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="01_Object"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:K10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:K10"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="01_Object Name"/>
     <tableColumn id="2" name="02_Type"/>
     <tableColumn id="3" name="03_Link to Specification" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" name="04_Developer"/>
-    <tableColumn id="5" name="05_Due Date" dataDxfId="0"/>
-    <tableColumn id="6" name="06_Sprint"/>
-    <tableColumn id="7" name="07_Ready for pct"/>
-    <tableColumn id="8" name="08_Dev Comment "/>
-    <tableColumn id="9" name="09_PM Comment"/>
+    <tableColumn id="11" name="05_Tasks"/>
+    <tableColumn id="5" name="06_Due Date" dataDxfId="0"/>
+    <tableColumn id="6" name="07_Sprint"/>
+    <tableColumn id="10" name="08_Status"/>
+    <tableColumn id="7" name="09_Ready for pct"/>
+    <tableColumn id="8" name="10_Dev Comment "/>
+    <tableColumn id="9" name="11_PM Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -448,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,153 +509,251 @@
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44803</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>0.85</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2">
-        <v>44803</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0.85</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2">
         <v>44803</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2">
         <v>44803</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
         <v>44803</v>
       </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2">
         <v>44803</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2">
+        <v>44803</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>0.95</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2">
+        <v>44803</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G4:G8">
+  <conditionalFormatting sqref="H4:I10">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -625,11 +773,14 @@
     <hyperlink ref="C6" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="C10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -645,7 +796,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G8</xm:sqref>
+          <xm:sqref>H4:I10</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
SR [2022-08-21]: PS Class <- transfer of mgm logic started
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planned Objects" sheetId="1" r:id="rId1"/>
-    <sheet name="Objects To Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Team" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Internet Sales</t>
   </si>
@@ -139,13 +139,79 @@
   </si>
   <si>
     <t>Waiting for specification</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>some_sample@email.com</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Amade Wolfgang</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Ledowskykh Sergii</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Shelly Bengia</t>
+  </si>
+  <si>
+    <t>sergii_razumov@epam.com</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>Razumov Sergii</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Report version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +226,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,19 +255,255 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
@@ -216,7 +524,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A3:K10" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PlannedObjects" displayName="PlannedObjects" ref="A3:K10" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A3:K10"/>
   <tableColumns count="11">
     <tableColumn id="1" name="01_Object Name"/>
@@ -224,12 +532,28 @@
     <tableColumn id="3" name="03_Link to Specification" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" name="04_Developer"/>
     <tableColumn id="11" name="05_Tasks"/>
-    <tableColumn id="5" name="06_Due Date" dataDxfId="0"/>
+    <tableColumn id="5" name="06_Due Date" dataDxfId="9"/>
     <tableColumn id="6" name="07_Sprint"/>
     <tableColumn id="10" name="08_Status"/>
     <tableColumn id="7" name="09_Ready for pct"/>
     <tableColumn id="8" name="10_Dev Comment "/>
     <tableColumn id="9" name="11_PM Comment"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="A3:G9"/>
+  <tableColumns count="7">
+    <tableColumn id="4" name="Index" dataDxfId="8"/>
+    <tableColumn id="5" name="Property" dataDxfId="7"/>
+    <tableColumn id="7" name="Value" dataDxfId="3"/>
+    <tableColumn id="2" name="Email" dataDxfId="1"/>
+    <tableColumn id="6" name="StartDate" dataDxfId="6"/>
+    <tableColumn id="3" name="EndDate" dataDxfId="2"/>
+    <tableColumn id="1" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -500,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,12 +1130,188 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6">
+        <v>44749</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="6">
+        <v>44749</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="6">
+        <v>44749</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="6">
+        <v>44749</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="6">
+        <v>44749</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="6">
+        <v>44749</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SR [2022-09-01]: Class Mgm method finished
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Planned Objects" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -264,7 +264,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -288,6 +288,58 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -391,7 +443,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -442,59 +494,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -544,15 +544,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A3:G9"/>
   <tableColumns count="7">
-    <tableColumn id="4" name="Index" dataDxfId="8"/>
-    <tableColumn id="5" name="Property" dataDxfId="7"/>
-    <tableColumn id="7" name="Value" dataDxfId="3"/>
-    <tableColumn id="2" name="Email" dataDxfId="1"/>
-    <tableColumn id="6" name="StartDate" dataDxfId="6"/>
-    <tableColumn id="3" name="EndDate" dataDxfId="2"/>
+    <tableColumn id="4" name="Index" dataDxfId="6"/>
+    <tableColumn id="5" name="Property" dataDxfId="5"/>
+    <tableColumn id="7" name="Value" dataDxfId="4"/>
+    <tableColumn id="2" name="Email" dataDxfId="3"/>
+    <tableColumn id="6" name="StartDate" dataDxfId="2"/>
+    <tableColumn id="3" name="EndDate" dataDxfId="1"/>
     <tableColumn id="1" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SR [2022-09-02]: Some bugs fixed --> update Specification in existing files, if smth is changed in mngm xls
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>Internet Sales</t>
   </si>
@@ -204,10 +204,19 @@
     <t>Report version</t>
   </si>
   <si>
-    <t>Some New Table</t>
-  </si>
-  <si>
     <t>NAN</t>
+  </si>
+  <si>
+    <t>Custom Internet Sales</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Removed from project on [2022-08-25] according to FUp letter from &lt;CustomerRepresentative&gt;</t>
+  </si>
+  <si>
+    <t>Some clarification is required!</t>
   </si>
 </sst>
 </file>
@@ -831,7 +840,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,6 +983,9 @@
       <c r="I6">
         <v>0.5</v>
       </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1084,31 +1096,31 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" t="s">
-        <v>37</v>
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SR [2022-09-06] Refactoring in Process --> adding to PS Class Build, Launch, WatchMode
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Planned Objects" sheetId="1" r:id="rId1"/>
     <sheet name="Team" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>Internet Sales</t>
   </si>
@@ -840,7 +841,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,7 +1181,7 @@
   <dimension ref="A3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,9 +1228,7 @@
       <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="6">
         <v>44749</v>
       </c>
@@ -1361,4 +1360,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SR [2022-09-21]: PS.MergeToMain() creds added
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planned Objects" sheetId="1" r:id="rId1"/>
     <sheet name="Team" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="PrivelegedUsers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>Internet Sales</t>
   </si>
@@ -169,9 +169,6 @@
     <t>some_sample@email.com</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>TL</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>QA</t>
   </si>
   <si>
-    <t>Report version</t>
-  </si>
-  <si>
     <t>NAN</t>
   </si>
   <si>
@@ -218,6 +212,18 @@
   </si>
   <si>
     <t>Some clarification is required!</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>MergeMain</t>
+  </si>
+  <si>
+    <t>sergiy.razumov@gmail.com</t>
+  </si>
+  <si>
+    <t>someemail@com</t>
   </si>
 </sst>
 </file>
@@ -560,8 +566,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A3:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A3:G8"/>
   <tableColumns count="7">
     <tableColumn id="4" name="Index" dataDxfId="6"/>
     <tableColumn id="5" name="Property" dataDxfId="5"/>
@@ -570,6 +576,17 @@
     <tableColumn id="6" name="StartDate" dataDxfId="2"/>
     <tableColumn id="3" name="EndDate" dataDxfId="1"/>
     <tableColumn id="1" name="Comment" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="PrivelegedUsers" displayName="PrivelegedUsers" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="User"/>
+    <tableColumn id="2" name="MergeMain"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -840,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -985,7 +1002,7 @@
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1097,31 +1114,31 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1178,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G9"/>
+  <dimension ref="A3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,15 +1237,17 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="E4" s="6">
         <v>44749</v>
       </c>
@@ -1241,13 +1260,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>46</v>
@@ -1264,13 +1283,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>46</v>
@@ -1287,16 +1306,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E7" s="6">
         <v>44749</v>
@@ -1310,16 +1329,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="6">
         <v>44749</v>
@@ -1328,29 +1347,6 @@
         <v>45</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="6">
-        <v>44749</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1364,12 +1360,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SR [2023-01-24]: Minor changes bf merging to Main
>> Minor Changes
</commit_message>
<xml_diff>
--- a/Management Plan.xlsx
+++ b/Management Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planned Objects" sheetId="1" r:id="rId1"/>
@@ -861,23 +861,23 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -912,7 +912,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -944,7 +944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1201,18 +1201,18 @@
       <selection activeCell="C4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -1366,12 +1366,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>

</xml_diff>